<commit_message>
update program of course
</commit_message>
<xml_diff>
--- a/Java-Basics-Course-Program-September-2015.xlsx
+++ b/Java-Basics-Course-Program-September-2015.xlsx
@@ -363,16 +363,16 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -463,7 +463,7 @@
   <dimension ref="1:16"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
+      <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2712,29 +2712,29 @@
         <v>42262</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" s="9" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="C9" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="D9" s="15" t="s">
+      <c r="D9" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="17" t="n">
+      <c r="E9" s="8" t="n">
         <v>42261</v>
       </c>
-      <c r="F9" s="17" t="s">
+      <c r="F9" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="17" t="s">
+      <c r="G9" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="H9" s="18" t="n">
+      <c r="H9" s="12" t="n">
         <v>42267</v>
       </c>
     </row>
@@ -2748,19 +2748,19 @@
       <c r="C10" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="D10" s="19" t="s">
+      <c r="D10" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="17" t="n">
+      <c r="E10" s="18" t="n">
         <v>42263</v>
       </c>
-      <c r="F10" s="17" t="s">
+      <c r="F10" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="G10" s="17" t="s">
+      <c r="G10" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="H10" s="18" t="n">
+      <c r="H10" s="19" t="n">
         <v>42269</v>
       </c>
     </row>
@@ -2777,16 +2777,16 @@
       <c r="D11" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="17" t="n">
+      <c r="E11" s="18" t="n">
         <v>42264</v>
       </c>
-      <c r="F11" s="17" t="s">
+      <c r="F11" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="G11" s="17" t="s">
+      <c r="G11" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="H11" s="18"/>
+      <c r="H11" s="19"/>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="n">
@@ -2801,16 +2801,16 @@
       <c r="D12" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="17" t="n">
+      <c r="E12" s="18" t="n">
         <v>42268</v>
       </c>
-      <c r="F12" s="17" t="s">
+      <c r="F12" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="G12" s="17" t="s">
+      <c r="G12" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="H12" s="18"/>
+      <c r="H12" s="19"/>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="n">
@@ -2822,19 +2822,19 @@
       <c r="C13" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="D13" s="19" t="s">
+      <c r="D13" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="E13" s="17" t="n">
+      <c r="E13" s="18" t="n">
         <v>42270</v>
       </c>
-      <c r="F13" s="17" t="s">
+      <c r="F13" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="G13" s="17" t="s">
+      <c r="G13" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="H13" s="18"/>
+      <c r="H13" s="19"/>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="s">
@@ -2849,16 +2849,16 @@
       <c r="D14" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="E14" s="17" t="n">
+      <c r="E14" s="18" t="n">
         <v>42272</v>
       </c>
-      <c r="F14" s="17" t="s">
+      <c r="F14" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="G14" s="17" t="s">
+      <c r="G14" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="H14" s="18"/>
+      <c r="H14" s="19"/>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="5" t="n">

</xml_diff>